<commit_message>
Small changes on contribution graphs
</commit_message>
<xml_diff>
--- a/data/data_minerals/USGS/Mineral_yearbook/myb1-2021-nickel-ERT.xlsx
+++ b/data/data_minerals/USGS/Mineral_yearbook/myb1-2021-nickel-ERT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/plca_metals_github/plca_metals/data/data_minerals/USGS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/plca_metals_github/plca_metals/data/data_minerals/USGS/Mineral_yearbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{59380E73-5D19-479F-BC66-0EF6DBC3C637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -3978,6 +3978,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4008,35 +4026,29 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4053,18 +4065,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -6740,12 +6740,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C6:Q6"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A4:U4"/>
-    <mergeCell ref="A5:U5"/>
     <mergeCell ref="A51:U51"/>
     <mergeCell ref="A52:U52"/>
     <mergeCell ref="A53:U53"/>
@@ -6756,6 +6750,12 @@
     <mergeCell ref="A48:U48"/>
     <mergeCell ref="A49:U49"/>
     <mergeCell ref="A50:U50"/>
+    <mergeCell ref="C6:Q6"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A4:U4"/>
+    <mergeCell ref="A5:U5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6789,80 +6789,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="274" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="284"/>
-      <c r="G1" s="284"/>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="284"/>
-      <c r="K1" s="284"/>
-      <c r="L1" s="284"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="274"/>
     </row>
     <row r="2" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="284" t="s">
+      <c r="A2" s="274" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
-      <c r="F2" s="284"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="284"/>
-      <c r="J2" s="284"/>
-      <c r="K2" s="284"/>
-      <c r="L2" s="284"/>
+      <c r="B2" s="274"/>
+      <c r="C2" s="274"/>
+      <c r="D2" s="274"/>
+      <c r="E2" s="274"/>
+      <c r="F2" s="274"/>
+      <c r="G2" s="274"/>
+      <c r="H2" s="274"/>
+      <c r="I2" s="274"/>
+      <c r="J2" s="274"/>
+      <c r="K2" s="274"/>
+      <c r="L2" s="274"/>
     </row>
     <row r="3" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="285"/>
-      <c r="B3" s="285"/>
-      <c r="C3" s="285"/>
-      <c r="D3" s="285"/>
-      <c r="E3" s="285"/>
-      <c r="F3" s="285"/>
-      <c r="G3" s="285"/>
-      <c r="H3" s="285"/>
-      <c r="I3" s="285"/>
-      <c r="J3" s="285"/>
-      <c r="K3" s="285"/>
-      <c r="L3" s="285"/>
+      <c r="A3" s="275"/>
+      <c r="B3" s="275"/>
+      <c r="C3" s="275"/>
+      <c r="D3" s="275"/>
+      <c r="E3" s="275"/>
+      <c r="F3" s="275"/>
+      <c r="G3" s="275"/>
+      <c r="H3" s="275"/>
+      <c r="I3" s="275"/>
+      <c r="J3" s="275"/>
+      <c r="K3" s="275"/>
+      <c r="L3" s="275"/>
     </row>
     <row r="4" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="284" t="s">
+      <c r="A4" s="274" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="284"/>
-      <c r="C4" s="284"/>
-      <c r="D4" s="284"/>
-      <c r="E4" s="284"/>
-      <c r="F4" s="284"/>
-      <c r="G4" s="284"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284"/>
-      <c r="J4" s="284"/>
-      <c r="K4" s="284"/>
-      <c r="L4" s="284"/>
+      <c r="B4" s="274"/>
+      <c r="C4" s="274"/>
+      <c r="D4" s="274"/>
+      <c r="E4" s="274"/>
+      <c r="F4" s="274"/>
+      <c r="G4" s="274"/>
+      <c r="H4" s="274"/>
+      <c r="I4" s="274"/>
+      <c r="J4" s="274"/>
+      <c r="K4" s="274"/>
+      <c r="L4" s="274"/>
     </row>
     <row r="5" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="286"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="287"/>
-      <c r="D5" s="287"/>
-      <c r="E5" s="287"/>
-      <c r="F5" s="287"/>
-      <c r="G5" s="287"/>
-      <c r="H5" s="287"/>
-      <c r="I5" s="287"/>
-      <c r="J5" s="287"/>
-      <c r="K5" s="287"/>
-      <c r="L5" s="287"/>
+      <c r="A5" s="276"/>
+      <c r="B5" s="277"/>
+      <c r="C5" s="277"/>
+      <c r="D5" s="277"/>
+      <c r="E5" s="277"/>
+      <c r="F5" s="277"/>
+      <c r="G5" s="277"/>
+      <c r="H5" s="277"/>
+      <c r="I5" s="277"/>
+      <c r="J5" s="277"/>
+      <c r="K5" s="277"/>
+      <c r="L5" s="277"/>
     </row>
     <row r="6" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="149" t="s">
@@ -7703,116 +7703,116 @@
       <c r="L40" s="169"/>
     </row>
     <row r="41" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="282" t="s">
+      <c r="A41" s="272" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="283"/>
-      <c r="C41" s="283"/>
-      <c r="D41" s="283"/>
-      <c r="E41" s="283"/>
-      <c r="F41" s="283"/>
-      <c r="G41" s="283"/>
-      <c r="H41" s="283"/>
-      <c r="I41" s="283"/>
-      <c r="J41" s="283"/>
-      <c r="K41" s="283"/>
-      <c r="L41" s="283"/>
+      <c r="B41" s="273"/>
+      <c r="C41" s="273"/>
+      <c r="D41" s="273"/>
+      <c r="E41" s="273"/>
+      <c r="F41" s="273"/>
+      <c r="G41" s="273"/>
+      <c r="H41" s="273"/>
+      <c r="I41" s="273"/>
+      <c r="J41" s="273"/>
+      <c r="K41" s="273"/>
+      <c r="L41" s="273"/>
     </row>
     <row r="42" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="272" t="s">
+      <c r="A42" s="278" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="273"/>
-      <c r="C42" s="273"/>
-      <c r="D42" s="273"/>
-      <c r="E42" s="273"/>
-      <c r="F42" s="273"/>
-      <c r="G42" s="273"/>
-      <c r="H42" s="273"/>
-      <c r="I42" s="273"/>
-      <c r="J42" s="273"/>
-      <c r="K42" s="273"/>
-      <c r="L42" s="273"/>
+      <c r="B42" s="279"/>
+      <c r="C42" s="279"/>
+      <c r="D42" s="279"/>
+      <c r="E42" s="279"/>
+      <c r="F42" s="279"/>
+      <c r="G42" s="279"/>
+      <c r="H42" s="279"/>
+      <c r="I42" s="279"/>
+      <c r="J42" s="279"/>
+      <c r="K42" s="279"/>
+      <c r="L42" s="279"/>
     </row>
     <row r="43" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="274" t="s">
+      <c r="A43" s="280" t="s">
         <v>302</v>
       </c>
-      <c r="B43" s="275"/>
-      <c r="C43" s="275"/>
-      <c r="D43" s="275"/>
-      <c r="E43" s="275"/>
-      <c r="F43" s="275"/>
-      <c r="G43" s="275"/>
-      <c r="H43" s="275"/>
-      <c r="I43" s="275"/>
-      <c r="J43" s="275"/>
-      <c r="K43" s="275"/>
-      <c r="L43" s="275"/>
+      <c r="B43" s="281"/>
+      <c r="C43" s="281"/>
+      <c r="D43" s="281"/>
+      <c r="E43" s="281"/>
+      <c r="F43" s="281"/>
+      <c r="G43" s="281"/>
+      <c r="H43" s="281"/>
+      <c r="I43" s="281"/>
+      <c r="J43" s="281"/>
+      <c r="K43" s="281"/>
+      <c r="L43" s="281"/>
     </row>
     <row r="44" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="276" t="s">
+      <c r="A44" s="282" t="s">
         <v>134</v>
       </c>
-      <c r="B44" s="277"/>
-      <c r="C44" s="277"/>
-      <c r="D44" s="277"/>
-      <c r="E44" s="277"/>
-      <c r="F44" s="277"/>
-      <c r="G44" s="277"/>
-      <c r="H44" s="277"/>
-      <c r="I44" s="277"/>
-      <c r="J44" s="277"/>
-      <c r="K44" s="277"/>
-      <c r="L44" s="277"/>
+      <c r="B44" s="283"/>
+      <c r="C44" s="283"/>
+      <c r="D44" s="283"/>
+      <c r="E44" s="283"/>
+      <c r="F44" s="283"/>
+      <c r="G44" s="283"/>
+      <c r="H44" s="283"/>
+      <c r="I44" s="283"/>
+      <c r="J44" s="283"/>
+      <c r="K44" s="283"/>
+      <c r="L44" s="283"/>
     </row>
     <row r="45" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="278" t="s">
+      <c r="A45" s="284" t="s">
         <v>324</v>
       </c>
-      <c r="B45" s="279"/>
-      <c r="C45" s="279"/>
-      <c r="D45" s="279"/>
-      <c r="E45" s="279"/>
-      <c r="F45" s="279"/>
-      <c r="G45" s="279"/>
-      <c r="H45" s="279"/>
-      <c r="I45" s="279"/>
-      <c r="J45" s="279"/>
-      <c r="K45" s="279"/>
-      <c r="L45" s="279"/>
+      <c r="B45" s="285"/>
+      <c r="C45" s="285"/>
+      <c r="D45" s="285"/>
+      <c r="E45" s="285"/>
+      <c r="F45" s="285"/>
+      <c r="G45" s="285"/>
+      <c r="H45" s="285"/>
+      <c r="I45" s="285"/>
+      <c r="J45" s="285"/>
+      <c r="K45" s="285"/>
+      <c r="L45" s="285"/>
     </row>
     <row r="46" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="280" t="s">
+      <c r="A46" s="286" t="s">
         <v>325</v>
       </c>
-      <c r="B46" s="281"/>
-      <c r="C46" s="281"/>
-      <c r="D46" s="281"/>
-      <c r="E46" s="281"/>
-      <c r="F46" s="281"/>
-      <c r="G46" s="281"/>
-      <c r="H46" s="281"/>
-      <c r="I46" s="281"/>
-      <c r="J46" s="281"/>
-      <c r="K46" s="281"/>
-      <c r="L46" s="281"/>
+      <c r="B46" s="287"/>
+      <c r="C46" s="287"/>
+      <c r="D46" s="287"/>
+      <c r="E46" s="287"/>
+      <c r="F46" s="287"/>
+      <c r="G46" s="287"/>
+      <c r="H46" s="287"/>
+      <c r="I46" s="287"/>
+      <c r="J46" s="287"/>
+      <c r="K46" s="287"/>
+      <c r="L46" s="287"/>
     </row>
     <row r="47" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="A46:L46"/>
     <mergeCell ref="A41:L41"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="A45:L45"/>
-    <mergeCell ref="A46:L46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -7845,80 +7845,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="274" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
-      <c r="E1" s="284"/>
-      <c r="F1" s="284"/>
-      <c r="G1" s="284"/>
-      <c r="H1" s="284"/>
-      <c r="I1" s="284"/>
-      <c r="J1" s="284"/>
-      <c r="K1" s="284"/>
-      <c r="L1" s="290"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="289"/>
     </row>
     <row r="2" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="284" t="s">
+      <c r="A2" s="274" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
-      <c r="F2" s="284"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="284"/>
-      <c r="J2" s="284"/>
-      <c r="K2" s="284"/>
-      <c r="L2" s="290"/>
+      <c r="B2" s="274"/>
+      <c r="C2" s="274"/>
+      <c r="D2" s="274"/>
+      <c r="E2" s="274"/>
+      <c r="F2" s="274"/>
+      <c r="G2" s="274"/>
+      <c r="H2" s="274"/>
+      <c r="I2" s="274"/>
+      <c r="J2" s="274"/>
+      <c r="K2" s="274"/>
+      <c r="L2" s="289"/>
     </row>
     <row r="3" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="285"/>
-      <c r="B3" s="285"/>
-      <c r="C3" s="285"/>
-      <c r="D3" s="285"/>
-      <c r="E3" s="285"/>
-      <c r="F3" s="285"/>
-      <c r="G3" s="285"/>
-      <c r="H3" s="285"/>
-      <c r="I3" s="285"/>
-      <c r="J3" s="285"/>
-      <c r="K3" s="285"/>
-      <c r="L3" s="290"/>
+      <c r="A3" s="275"/>
+      <c r="B3" s="275"/>
+      <c r="C3" s="275"/>
+      <c r="D3" s="275"/>
+      <c r="E3" s="275"/>
+      <c r="F3" s="275"/>
+      <c r="G3" s="275"/>
+      <c r="H3" s="275"/>
+      <c r="I3" s="275"/>
+      <c r="J3" s="275"/>
+      <c r="K3" s="275"/>
+      <c r="L3" s="289"/>
     </row>
     <row r="4" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="284" t="s">
+      <c r="A4" s="274" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="284"/>
-      <c r="C4" s="284"/>
-      <c r="D4" s="284"/>
-      <c r="E4" s="284"/>
-      <c r="F4" s="284"/>
-      <c r="G4" s="284"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284"/>
-      <c r="J4" s="284"/>
-      <c r="K4" s="284"/>
-      <c r="L4" s="290"/>
+      <c r="B4" s="274"/>
+      <c r="C4" s="274"/>
+      <c r="D4" s="274"/>
+      <c r="E4" s="274"/>
+      <c r="F4" s="274"/>
+      <c r="G4" s="274"/>
+      <c r="H4" s="274"/>
+      <c r="I4" s="274"/>
+      <c r="J4" s="274"/>
+      <c r="K4" s="274"/>
+      <c r="L4" s="289"/>
     </row>
     <row r="5" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="286"/>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="286"/>
-      <c r="H5" s="286"/>
-      <c r="I5" s="286"/>
-      <c r="J5" s="286"/>
-      <c r="K5" s="286"/>
-      <c r="L5" s="291"/>
+      <c r="A5" s="276"/>
+      <c r="B5" s="276"/>
+      <c r="C5" s="276"/>
+      <c r="D5" s="276"/>
+      <c r="E5" s="276"/>
+      <c r="F5" s="276"/>
+      <c r="G5" s="276"/>
+      <c r="H5" s="276"/>
+      <c r="I5" s="276"/>
+      <c r="J5" s="276"/>
+      <c r="K5" s="276"/>
+      <c r="L5" s="290"/>
     </row>
     <row r="6" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="149" t="s">
@@ -8362,159 +8362,153 @@
       <c r="L24" s="168"/>
     </row>
     <row r="25" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="289" t="s">
+      <c r="A25" s="288" t="s">
         <v>254</v>
       </c>
-      <c r="B25" s="289"/>
-      <c r="C25" s="289"/>
-      <c r="D25" s="289"/>
-      <c r="E25" s="289"/>
-      <c r="F25" s="289"/>
-      <c r="G25" s="289"/>
-      <c r="H25" s="289"/>
-      <c r="I25" s="289"/>
-      <c r="J25" s="289"/>
-      <c r="K25" s="289"/>
-      <c r="L25" s="289"/>
+      <c r="B25" s="288"/>
+      <c r="C25" s="288"/>
+      <c r="D25" s="288"/>
+      <c r="E25" s="288"/>
+      <c r="F25" s="288"/>
+      <c r="G25" s="288"/>
+      <c r="H25" s="288"/>
+      <c r="I25" s="288"/>
+      <c r="J25" s="288"/>
+      <c r="K25" s="288"/>
+      <c r="L25" s="288"/>
     </row>
     <row r="26" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="272" t="s">
+      <c r="A26" s="278" t="s">
         <v>255</v>
       </c>
-      <c r="B26" s="272"/>
-      <c r="C26" s="272"/>
-      <c r="D26" s="272"/>
-      <c r="E26" s="272"/>
-      <c r="F26" s="272"/>
-      <c r="G26" s="272"/>
-      <c r="H26" s="272"/>
-      <c r="I26" s="272"/>
-      <c r="J26" s="272"/>
-      <c r="K26" s="272"/>
-      <c r="L26" s="288"/>
+      <c r="B26" s="278"/>
+      <c r="C26" s="278"/>
+      <c r="D26" s="278"/>
+      <c r="E26" s="278"/>
+      <c r="F26" s="278"/>
+      <c r="G26" s="278"/>
+      <c r="H26" s="278"/>
+      <c r="I26" s="278"/>
+      <c r="J26" s="278"/>
+      <c r="K26" s="278"/>
+      <c r="L26" s="291"/>
     </row>
     <row r="27" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="289" t="s">
+      <c r="A27" s="288" t="s">
         <v>256</v>
       </c>
-      <c r="B27" s="289"/>
-      <c r="C27" s="289"/>
-      <c r="D27" s="289"/>
-      <c r="E27" s="289"/>
-      <c r="F27" s="289"/>
-      <c r="G27" s="289"/>
-      <c r="H27" s="289"/>
-      <c r="I27" s="289"/>
-      <c r="J27" s="289"/>
-      <c r="K27" s="289"/>
-      <c r="L27" s="288"/>
+      <c r="B27" s="288"/>
+      <c r="C27" s="288"/>
+      <c r="D27" s="288"/>
+      <c r="E27" s="288"/>
+      <c r="F27" s="288"/>
+      <c r="G27" s="288"/>
+      <c r="H27" s="288"/>
+      <c r="I27" s="288"/>
+      <c r="J27" s="288"/>
+      <c r="K27" s="288"/>
+      <c r="L27" s="291"/>
     </row>
     <row r="28" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="276" t="s">
+      <c r="A28" s="282" t="s">
         <v>257</v>
       </c>
-      <c r="B28" s="276"/>
-      <c r="C28" s="276"/>
-      <c r="D28" s="276"/>
-      <c r="E28" s="276"/>
-      <c r="F28" s="276"/>
-      <c r="G28" s="276"/>
-      <c r="H28" s="276"/>
-      <c r="I28" s="276"/>
-      <c r="J28" s="276"/>
-      <c r="K28" s="276"/>
-      <c r="L28" s="288"/>
+      <c r="B28" s="282"/>
+      <c r="C28" s="282"/>
+      <c r="D28" s="282"/>
+      <c r="E28" s="282"/>
+      <c r="F28" s="282"/>
+      <c r="G28" s="282"/>
+      <c r="H28" s="282"/>
+      <c r="I28" s="282"/>
+      <c r="J28" s="282"/>
+      <c r="K28" s="282"/>
+      <c r="L28" s="291"/>
     </row>
     <row r="29" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="276" t="s">
+      <c r="A29" s="282" t="s">
         <v>258</v>
       </c>
-      <c r="B29" s="276"/>
-      <c r="C29" s="276"/>
-      <c r="D29" s="276"/>
-      <c r="E29" s="276"/>
-      <c r="F29" s="276"/>
-      <c r="G29" s="276"/>
-      <c r="H29" s="276"/>
-      <c r="I29" s="276"/>
-      <c r="J29" s="276"/>
-      <c r="K29" s="276"/>
-      <c r="L29" s="288"/>
+      <c r="B29" s="282"/>
+      <c r="C29" s="282"/>
+      <c r="D29" s="282"/>
+      <c r="E29" s="282"/>
+      <c r="F29" s="282"/>
+      <c r="G29" s="282"/>
+      <c r="H29" s="282"/>
+      <c r="I29" s="282"/>
+      <c r="J29" s="282"/>
+      <c r="K29" s="282"/>
+      <c r="L29" s="291"/>
     </row>
     <row r="30" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="276" t="s">
+      <c r="A30" s="282" t="s">
         <v>259</v>
       </c>
-      <c r="B30" s="276"/>
-      <c r="C30" s="276"/>
-      <c r="D30" s="276"/>
-      <c r="E30" s="276"/>
-      <c r="F30" s="276"/>
-      <c r="G30" s="276"/>
-      <c r="H30" s="276"/>
-      <c r="I30" s="276"/>
-      <c r="J30" s="276"/>
-      <c r="K30" s="276"/>
-      <c r="L30" s="288"/>
+      <c r="B30" s="282"/>
+      <c r="C30" s="282"/>
+      <c r="D30" s="282"/>
+      <c r="E30" s="282"/>
+      <c r="F30" s="282"/>
+      <c r="G30" s="282"/>
+      <c r="H30" s="282"/>
+      <c r="I30" s="282"/>
+      <c r="J30" s="282"/>
+      <c r="K30" s="282"/>
+      <c r="L30" s="291"/>
     </row>
     <row r="31" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="280" t="s">
+      <c r="A31" s="286" t="s">
         <v>260</v>
       </c>
-      <c r="B31" s="280"/>
-      <c r="C31" s="280"/>
-      <c r="D31" s="280"/>
-      <c r="E31" s="280"/>
-      <c r="F31" s="280"/>
-      <c r="G31" s="280"/>
-      <c r="H31" s="280"/>
-      <c r="I31" s="280"/>
-      <c r="J31" s="280"/>
-      <c r="K31" s="280"/>
-      <c r="L31" s="288"/>
+      <c r="B31" s="286"/>
+      <c r="C31" s="286"/>
+      <c r="D31" s="286"/>
+      <c r="E31" s="286"/>
+      <c r="F31" s="286"/>
+      <c r="G31" s="286"/>
+      <c r="H31" s="286"/>
+      <c r="I31" s="286"/>
+      <c r="J31" s="286"/>
+      <c r="K31" s="286"/>
+      <c r="L31" s="291"/>
     </row>
     <row r="32" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="280" t="s">
+      <c r="A32" s="286" t="s">
         <v>261</v>
       </c>
-      <c r="B32" s="280"/>
-      <c r="C32" s="280"/>
-      <c r="D32" s="280"/>
-      <c r="E32" s="280"/>
-      <c r="F32" s="280"/>
-      <c r="G32" s="280"/>
-      <c r="H32" s="280"/>
-      <c r="I32" s="280"/>
-      <c r="J32" s="280"/>
-      <c r="K32" s="280"/>
-      <c r="L32" s="288"/>
+      <c r="B32" s="286"/>
+      <c r="C32" s="286"/>
+      <c r="D32" s="286"/>
+      <c r="E32" s="286"/>
+      <c r="F32" s="286"/>
+      <c r="G32" s="286"/>
+      <c r="H32" s="286"/>
+      <c r="I32" s="286"/>
+      <c r="J32" s="286"/>
+      <c r="K32" s="286"/>
+      <c r="L32" s="291"/>
     </row>
     <row r="33" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="280" t="s">
+      <c r="A33" s="286" t="s">
         <v>262</v>
       </c>
-      <c r="B33" s="280"/>
-      <c r="C33" s="280"/>
-      <c r="D33" s="280"/>
-      <c r="E33" s="280"/>
-      <c r="F33" s="280"/>
-      <c r="G33" s="280"/>
-      <c r="H33" s="280"/>
-      <c r="I33" s="280"/>
-      <c r="J33" s="280"/>
-      <c r="K33" s="280"/>
-      <c r="L33" s="288"/>
+      <c r="B33" s="286"/>
+      <c r="C33" s="286"/>
+      <c r="D33" s="286"/>
+      <c r="E33" s="286"/>
+      <c r="F33" s="286"/>
+      <c r="G33" s="286"/>
+      <c r="H33" s="286"/>
+      <c r="I33" s="286"/>
+      <c r="J33" s="286"/>
+      <c r="K33" s="286"/>
+      <c r="L33" s="291"/>
     </row>
     <row r="34" spans="1:12" ht="10.199999999999999" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:12" ht="10.199999999999999" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
     <mergeCell ref="A32:L32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="A26:L26"/>
@@ -8523,6 +8517,12 @@
     <mergeCell ref="A29:L29"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8534,8 +8534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40AB4B3-01FF-44DE-9397-27AA552084B4}">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8555,80 +8555,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="180" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="293" t="s">
+      <c r="A1" s="296" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="293"/>
-      <c r="C1" s="293"/>
-      <c r="D1" s="293"/>
-      <c r="E1" s="293"/>
-      <c r="F1" s="293"/>
-      <c r="G1" s="293"/>
-      <c r="H1" s="293"/>
-      <c r="I1" s="293"/>
-      <c r="J1" s="293"/>
-      <c r="K1" s="293"/>
-      <c r="L1" s="293"/>
+      <c r="B1" s="296"/>
+      <c r="C1" s="296"/>
+      <c r="D1" s="296"/>
+      <c r="E1" s="296"/>
+      <c r="F1" s="296"/>
+      <c r="G1" s="296"/>
+      <c r="H1" s="296"/>
+      <c r="I1" s="296"/>
+      <c r="J1" s="296"/>
+      <c r="K1" s="296"/>
+      <c r="L1" s="296"/>
     </row>
     <row r="2" spans="1:12" s="180" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="293" t="s">
+      <c r="A2" s="296" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="293"/>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293"/>
-      <c r="H2" s="293"/>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
+      <c r="B2" s="296"/>
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="296"/>
+      <c r="I2" s="296"/>
+      <c r="J2" s="296"/>
+      <c r="K2" s="296"/>
+      <c r="L2" s="296"/>
     </row>
     <row r="3" spans="1:12" s="180" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="294"/>
-      <c r="B3" s="294"/>
-      <c r="C3" s="294"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294"/>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
+      <c r="A3" s="297"/>
+      <c r="B3" s="297"/>
+      <c r="C3" s="297"/>
+      <c r="D3" s="297"/>
+      <c r="E3" s="297"/>
+      <c r="F3" s="297"/>
+      <c r="G3" s="297"/>
+      <c r="H3" s="297"/>
+      <c r="I3" s="297"/>
+      <c r="J3" s="297"/>
+      <c r="K3" s="297"/>
+      <c r="L3" s="297"/>
     </row>
     <row r="4" spans="1:12" s="180" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="293" t="s">
+      <c r="A4" s="296" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="293"/>
-      <c r="C4" s="293"/>
-      <c r="D4" s="293"/>
-      <c r="E4" s="293"/>
-      <c r="F4" s="293"/>
-      <c r="G4" s="293"/>
-      <c r="H4" s="293"/>
-      <c r="I4" s="293"/>
-      <c r="J4" s="293"/>
-      <c r="K4" s="293"/>
-      <c r="L4" s="293"/>
+      <c r="B4" s="296"/>
+      <c r="C4" s="296"/>
+      <c r="D4" s="296"/>
+      <c r="E4" s="296"/>
+      <c r="F4" s="296"/>
+      <c r="G4" s="296"/>
+      <c r="H4" s="296"/>
+      <c r="I4" s="296"/>
+      <c r="J4" s="296"/>
+      <c r="K4" s="296"/>
+      <c r="L4" s="296"/>
     </row>
     <row r="5" spans="1:12" s="180" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="295"/>
-      <c r="B5" s="296"/>
-      <c r="C5" s="296"/>
-      <c r="D5" s="296"/>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
-      <c r="G5" s="296"/>
-      <c r="H5" s="296"/>
-      <c r="I5" s="296"/>
-      <c r="J5" s="296"/>
-      <c r="K5" s="296"/>
-      <c r="L5" s="296"/>
+      <c r="A5" s="298"/>
+      <c r="B5" s="299"/>
+      <c r="C5" s="299"/>
+      <c r="D5" s="299"/>
+      <c r="E5" s="299"/>
+      <c r="F5" s="299"/>
+      <c r="G5" s="299"/>
+      <c r="H5" s="299"/>
+      <c r="I5" s="299"/>
+      <c r="J5" s="299"/>
+      <c r="K5" s="299"/>
+      <c r="L5" s="299"/>
     </row>
     <row r="6" spans="1:12" s="180" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="181" t="s">
@@ -10145,52 +10145,52 @@
       <c r="L64" s="192"/>
     </row>
     <row r="65" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="292" t="s">
+      <c r="A65" s="295" t="s">
         <v>132</v>
       </c>
-      <c r="B65" s="292"/>
-      <c r="C65" s="292"/>
-      <c r="D65" s="292"/>
-      <c r="E65" s="292"/>
-      <c r="F65" s="292"/>
-      <c r="G65" s="292"/>
-      <c r="H65" s="292"/>
-      <c r="I65" s="292"/>
-      <c r="J65" s="292"/>
-      <c r="K65" s="292"/>
-      <c r="L65" s="292"/>
+      <c r="B65" s="295"/>
+      <c r="C65" s="295"/>
+      <c r="D65" s="295"/>
+      <c r="E65" s="295"/>
+      <c r="F65" s="295"/>
+      <c r="G65" s="295"/>
+      <c r="H65" s="295"/>
+      <c r="I65" s="295"/>
+      <c r="J65" s="295"/>
+      <c r="K65" s="295"/>
+      <c r="L65" s="295"/>
     </row>
     <row r="66" spans="1:12" s="180" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="298" t="s">
+      <c r="A66" s="293" t="s">
         <v>296</v>
       </c>
-      <c r="B66" s="298"/>
-      <c r="C66" s="298"/>
-      <c r="D66" s="298"/>
-      <c r="E66" s="298"/>
-      <c r="F66" s="298"/>
-      <c r="G66" s="298"/>
-      <c r="H66" s="298"/>
-      <c r="I66" s="298"/>
-      <c r="J66" s="298"/>
-      <c r="K66" s="298"/>
-      <c r="L66" s="298"/>
+      <c r="B66" s="293"/>
+      <c r="C66" s="293"/>
+      <c r="D66" s="293"/>
+      <c r="E66" s="293"/>
+      <c r="F66" s="293"/>
+      <c r="G66" s="293"/>
+      <c r="H66" s="293"/>
+      <c r="I66" s="293"/>
+      <c r="J66" s="293"/>
+      <c r="K66" s="293"/>
+      <c r="L66" s="293"/>
     </row>
     <row r="67" spans="1:12" s="185" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="299" t="s">
+      <c r="A67" s="294" t="s">
         <v>297</v>
       </c>
-      <c r="B67" s="299"/>
-      <c r="C67" s="299"/>
-      <c r="D67" s="299"/>
-      <c r="E67" s="299"/>
-      <c r="F67" s="299"/>
-      <c r="G67" s="299"/>
-      <c r="H67" s="299"/>
-      <c r="I67" s="299"/>
-      <c r="J67" s="299"/>
-      <c r="K67" s="299"/>
-      <c r="L67" s="299"/>
+      <c r="B67" s="294"/>
+      <c r="C67" s="294"/>
+      <c r="D67" s="294"/>
+      <c r="E67" s="294"/>
+      <c r="F67" s="294"/>
+      <c r="G67" s="294"/>
+      <c r="H67" s="294"/>
+      <c r="I67" s="294"/>
+      <c r="J67" s="294"/>
+      <c r="K67" s="294"/>
+      <c r="L67" s="294"/>
     </row>
     <row r="68" spans="1:12" s="180" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="265" t="s">
@@ -10209,71 +10209,77 @@
       <c r="L68" s="265"/>
     </row>
     <row r="69" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="297" t="s">
+      <c r="A69" s="292" t="s">
         <v>341</v>
       </c>
-      <c r="B69" s="297"/>
-      <c r="C69" s="297"/>
-      <c r="D69" s="297"/>
-      <c r="E69" s="297"/>
-      <c r="F69" s="297"/>
-      <c r="G69" s="297"/>
-      <c r="H69" s="297"/>
-      <c r="I69" s="297"/>
-      <c r="J69" s="297"/>
-      <c r="K69" s="297"/>
-      <c r="L69" s="297"/>
+      <c r="B69" s="292"/>
+      <c r="C69" s="292"/>
+      <c r="D69" s="292"/>
+      <c r="E69" s="292"/>
+      <c r="F69" s="292"/>
+      <c r="G69" s="292"/>
+      <c r="H69" s="292"/>
+      <c r="I69" s="292"/>
+      <c r="J69" s="292"/>
+      <c r="K69" s="292"/>
+      <c r="L69" s="292"/>
     </row>
     <row r="70" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="297" t="s">
+      <c r="A70" s="292" t="s">
         <v>342</v>
       </c>
-      <c r="B70" s="297"/>
-      <c r="C70" s="297"/>
-      <c r="D70" s="297"/>
-      <c r="E70" s="297"/>
-      <c r="F70" s="297"/>
-      <c r="G70" s="297"/>
-      <c r="H70" s="297"/>
-      <c r="I70" s="297"/>
-      <c r="J70" s="297"/>
-      <c r="K70" s="297"/>
-      <c r="L70" s="297"/>
+      <c r="B70" s="292"/>
+      <c r="C70" s="292"/>
+      <c r="D70" s="292"/>
+      <c r="E70" s="292"/>
+      <c r="F70" s="292"/>
+      <c r="G70" s="292"/>
+      <c r="H70" s="292"/>
+      <c r="I70" s="292"/>
+      <c r="J70" s="292"/>
+      <c r="K70" s="292"/>
+      <c r="L70" s="292"/>
     </row>
     <row r="71" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="297" t="s">
+      <c r="A71" s="292" t="s">
         <v>343</v>
       </c>
-      <c r="B71" s="297"/>
-      <c r="C71" s="297"/>
-      <c r="D71" s="297"/>
-      <c r="E71" s="297"/>
-      <c r="F71" s="297"/>
-      <c r="G71" s="297"/>
-      <c r="H71" s="297"/>
-      <c r="I71" s="297"/>
-      <c r="J71" s="297"/>
-      <c r="K71" s="297"/>
-      <c r="L71" s="297"/>
+      <c r="B71" s="292"/>
+      <c r="C71" s="292"/>
+      <c r="D71" s="292"/>
+      <c r="E71" s="292"/>
+      <c r="F71" s="292"/>
+      <c r="G71" s="292"/>
+      <c r="H71" s="292"/>
+      <c r="I71" s="292"/>
+      <c r="J71" s="292"/>
+      <c r="K71" s="292"/>
+      <c r="L71" s="292"/>
     </row>
     <row r="72" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="297" t="s">
+      <c r="A72" s="292" t="s">
         <v>344</v>
       </c>
-      <c r="B72" s="297"/>
-      <c r="C72" s="297"/>
-      <c r="D72" s="297"/>
-      <c r="E72" s="297"/>
-      <c r="F72" s="297"/>
-      <c r="G72" s="297"/>
-      <c r="H72" s="297"/>
-      <c r="I72" s="297"/>
-      <c r="J72" s="297"/>
-      <c r="K72" s="297"/>
-      <c r="L72" s="297"/>
+      <c r="B72" s="292"/>
+      <c r="C72" s="292"/>
+      <c r="D72" s="292"/>
+      <c r="E72" s="292"/>
+      <c r="F72" s="292"/>
+      <c r="G72" s="292"/>
+      <c r="H72" s="292"/>
+      <c r="I72" s="292"/>
+      <c r="J72" s="292"/>
+      <c r="K72" s="292"/>
+      <c r="L72" s="292"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
     <mergeCell ref="A72:L72"/>
     <mergeCell ref="A66:L66"/>
     <mergeCell ref="A67:L67"/>
@@ -10281,12 +10287,6 @@
     <mergeCell ref="A69:L69"/>
     <mergeCell ref="A70:L70"/>
     <mergeCell ref="A71:L71"/>
-    <mergeCell ref="A65:L65"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11761,17 +11761,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15728,12 +15728,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C6:Q6"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="A4:U4"/>
-    <mergeCell ref="A5:U5"/>
     <mergeCell ref="A52:U52"/>
     <mergeCell ref="A53:U53"/>
     <mergeCell ref="A54:U54"/>
@@ -15744,6 +15738,12 @@
     <mergeCell ref="A49:U49"/>
     <mergeCell ref="A50:U50"/>
     <mergeCell ref="A51:U51"/>
+    <mergeCell ref="C6:Q6"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A4:U4"/>
+    <mergeCell ref="A5:U5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16544,12 +16544,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
     <mergeCell ref="A43:I43"/>
     <mergeCell ref="A36:I36"/>
     <mergeCell ref="A38:I38"/>
@@ -16558,6 +16552,12 @@
     <mergeCell ref="A41:I41"/>
     <mergeCell ref="A42:I42"/>
     <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>